<commit_message>
words used from glossary
</commit_message>
<xml_diff>
--- a/glossary_ur.xlsx
+++ b/glossary_ur.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,37 +453,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>crypto</t>
+          <t>in</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>کرپٹو</t>
+          <t>میں</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>crypto</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>پروجیکٹ</t>
+          <t>کرپٹو</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>therapy</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -491,14 +491,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>تھراپی</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>to</t>
+          <t>activities</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -506,104 +506,104 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>کو</t>
+          <t>سرگرمیاں</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>s</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>تاریخ</t>
+          <t>ایس</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>autonomous</t>
+          <t>assessment</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>خود مختار</t>
+          <t>تشخیص</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>journalist</t>
+          <t>project</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>صحافی</t>
+          <t>پروجیکٹ</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>and</t>
+          <t>occupational</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>اور</t>
+          <t>پیشہ ورانہ</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>we</t>
+          <t>to</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ہم</t>
+          <t>کو</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>agent</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ایجنٹ</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>phase</t>
+          <t>we</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -611,179 +611,179 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>مرحلہ</t>
+          <t>ہم</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>company</t>
+          <t>personal</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>کمپنی</t>
+          <t>ذاتی</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>that</t>
+          <t>date</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>وہ</t>
+          <t>تاریخ</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>an</t>
+          <t>agent</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ایک</t>
+          <t>ایجنٹ</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>build</t>
+          <t>autonomous</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>تعمیر کریں</t>
+          <t>خود مختار</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>aim</t>
+          <t>journalist</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>مقصد</t>
+          <t>صحافی</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>overview</t>
+          <t>and</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>جائزہ</t>
+          <t>اور</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>needs</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>۰</t>
+          <t>ضروریات</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>her</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>نام</t>
+          <t>اس کی</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>your</t>
+          <t>with</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>آپ کا</t>
+          <t>کے ساتھ</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>author</t>
+          <t>this</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>مصنف</t>
+          <t>یہ</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>insert</t>
+          <t>phase</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>داخل کریں</t>
+          <t>مرحلہ</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>real</t>
+          <t>engage</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -791,14 +791,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>حقیقی</t>
+          <t>مشغول</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>everyday</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -806,14 +806,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ورژن</t>
+          <t>روزمرہ</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>gathers</t>
+          <t>academic</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -821,14 +821,14 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>جمع کرتا ہے</t>
+          <t>علمی</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>blockchain</t>
+          <t>all</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -836,14 +836,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>بلاک چین</t>
+          <t>سب</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>relating</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -851,14 +851,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>وقت</t>
+          <t>متعلق</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>information</t>
+          <t>progress</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -866,14 +866,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>معلومات</t>
+          <t>ترقی</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>from</t>
+          <t>learn</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -881,14 +881,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>سے</t>
+          <t>سیکھنا</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>various</t>
+          <t>access</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -896,14 +896,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>مختلف</t>
+          <t>رسائی</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>of</t>
+          <t>adequately</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -911,14 +911,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>کا</t>
+          <t>مناسب طور پر</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sources</t>
+          <t>enable</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -926,14 +926,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ذرائع</t>
+          <t>فعال کریں</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>objectively</t>
+          <t>place</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -941,14 +941,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>معروضی طور پر</t>
+          <t>جگہ</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -956,14 +956,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>عنوان</t>
+          <t>سیکھنا</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>on</t>
+          <t>be</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -971,14 +971,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>پر</t>
+          <t>ہونا</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>what</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -986,14 +986,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>یہ</t>
+          <t>کیا</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>soon</t>
+          <t>care</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1001,14 +1001,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>جلد</t>
+          <t>دیکھ بھال</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>as</t>
+          <t>play</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1016,14 +1016,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>بطور</t>
+          <t>کھیلنا</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>its</t>
+          <t>independence</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1031,14 +1031,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>اس کا</t>
+          <t>آزادی</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>started</t>
+          <t>interaction</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1046,14 +1046,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>شروع کیا</t>
+          <t>تفاعل</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>functional</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1061,14 +1061,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>کام کر رہا ہے</t>
+          <t>فعال</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>work</t>
+          <t>perceptual</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1076,14 +1076,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>کام</t>
+          <t>ادراکی</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>transactions</t>
+          <t>sensory</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1091,14 +1091,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>لین دین</t>
+          <t>حسی</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>statement</t>
+          <t>functioning</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1106,14 +1106,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>بیان</t>
+          <t>فعال</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>across</t>
+          <t>motor</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1121,14 +1121,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>پار</t>
+          <t>موٹر</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>xx</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1136,14 +1136,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ایک</t>
+          <t>ایکس ایکس</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>eventually</t>
+          <t>at</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1151,14 +1151,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>بالآخر</t>
+          <t>پر</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>integrates</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1166,14 +1166,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ضم کرتا ہے</t>
+          <t>گھر</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>payment</t>
+          <t>impact</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1181,14 +1181,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ادائیگی</t>
+          <t>اثر</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>functionality</t>
+          <t>analysing</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1196,14 +1196,14 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>فعالیت</t>
+          <t>تجزیہ کرنا</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>by</t>
+          <t>school</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1211,14 +1211,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>کی طرف سے</t>
+          <t>اسکول</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>splitting</t>
+          <t>focus</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1226,14 +1226,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>تقسیم</t>
+          <t>توجہ</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>the</t>
+          <t>participate</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1241,14 +1241,14 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>دی</t>
+          <t>حصہ لینا</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>into</t>
+          <t>demands</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1256,14 +1256,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>میں</t>
+          <t>مطالبات</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>two</t>
+          <t>ability</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1271,14 +1271,14 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>دو</t>
+          <t>صلاحیت</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>phases</t>
+          <t>expected</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1286,14 +1286,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>مراحل</t>
+          <t>متوقع</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>can</t>
+          <t>their</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1301,14 +1301,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>کر سکتا ہے</t>
+          <t>ان کا</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>establish</t>
+          <t>consist</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1316,14 +1316,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>قائم کرنا</t>
+          <t>مشتمل ہونا</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>strong</t>
+          <t>these</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1331,14 +1331,14 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>مضبوط</t>
+          <t>یہ</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>people</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1346,14 +1346,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>لوگ</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>journalistic</t>
+          <t>young</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1361,14 +1361,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>صحافتی</t>
+          <t>نوجوان</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>you</t>
+          <t>children</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1376,14 +1376,14 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>آپ</t>
+          <t>بچے</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>first</t>
+          <t>considered</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1391,14 +1391,14 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>پہلا</t>
+          <t>غور کیا گیا</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>see</t>
+          <t>primarily</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1406,14 +1406,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>دیکھنا</t>
+          <t>بنیادی طور پر</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>platforms</t>
+          <t>are</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1421,14 +1421,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>پلیٹ فارمز</t>
+          <t>ہیں</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>then</t>
+          <t>performance</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1436,14 +1436,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>پھر</t>
+          <t>کارکردگی</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>expand</t>
+          <t>tasks</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1451,14 +1451,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>پھیلانا</t>
+          <t>کام</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>include</t>
+          <t>life</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1466,14 +1466,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>شامل کریں</t>
+          <t>زندگی</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>wallet</t>
+          <t>daily</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1481,14 +1481,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>بٹوہ</t>
+          <t>روزانہ</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>based</t>
+          <t>out</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1496,14 +1496,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>مبنی بر</t>
+          <t>باہر</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>carry</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1511,14 +1511,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>اچھا</t>
+          <t>لے جانا</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>document</t>
+          <t>abilities</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1526,14 +1526,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>دستاویز</t>
+          <t>صلاحیتیں</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>reports</t>
+          <t>individual</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1541,14 +1541,14 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>رپورٹس</t>
+          <t>فرد</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>social</t>
+          <t>means</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1556,22 +1556,1252 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>سماجی</t>
+          <t>ذرائع</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>approach</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>قریب ہونا</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>نیچے</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>اوپر</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>follows</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>پیروی کرتا ہے</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>guidelines</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>رہنما اصول</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>cot</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>چارپائی</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>will</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>مرضی</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>لکیر</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>setting</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ترتیب</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>educational</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>تعلیمی</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>within</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>اندر</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>college</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>کالج</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>child</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>بچہ</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>father</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>والد</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>یہ</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>various</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>1</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>مختلف</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>of</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>کا</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>ذرائع</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>objectively</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>معروضی طور پر</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>عنوان</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>پر</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>soon</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>جلد</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>information</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>معلومات</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>as</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>بطور</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>its</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>اس کا</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>شروع کیا</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>کام کر رہا ہے</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>work</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>کام</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>transactions</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>لین دین</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>from</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>سے</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>وقت</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>requested</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>درخواست کی گئی</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>۰</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>company</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>کمپنی</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>that</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>وہ</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>an</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>ایک</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>build</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>تعمیر کریں</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>aim</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>مقصد</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>overview</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>1</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>جائزہ</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>نام</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>blockchain</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>بلاک چین</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>your</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>آپ کا</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>مصنف</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>insert</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>1</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>داخل کریں</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>حقیقی</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>ورژن</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>gathers</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>جمع کرتا ہے</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>statement</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>بیان</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>across</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>پار</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>ایک</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>اچھا</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>platforms</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>پلیٹ فارمز</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>then</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>پھر</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>expand</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>1</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>پھیلانا</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>include</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>1</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>شامل کریں</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>wallet</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>بٹوہ</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>based</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>1</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>مبنی بر</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>document</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>1</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>دستاویز</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>eventually</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>بالآخر</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>reports</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>1</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>رپورٹس</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>social</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>1</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>سماجی</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
           <t>properly</t>
         </is>
       </c>
-      <c r="B76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" t="inlineStr">
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" t="inlineStr">
         <is>
           <t>صحیح طریقے سے</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>رپورٹ</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>introduction</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>تعارف</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>was</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>تھا</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>see</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>دیکھنا</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>first</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>پہلا</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>you</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>آپ</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>journalistic</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>1</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>صحافتی</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>strong</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>مضبوط</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>establish</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>1</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>قائم کرنا</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>can</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>1</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>کر سکتا ہے</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>1</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>مراحل</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>two</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>1</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>دو</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>into</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>1</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>میں</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>دی</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>splitting</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>تقسیم</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>by</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>1</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>کی طرف سے</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>functionality</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>فعالیت</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>payment</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>ادائیگی</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>integrates</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>1</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>ضم کرتا ہے</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>community</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>1</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>کمیونٹی</t>
         </is>
       </c>
     </row>

</xml_diff>